<commit_message>
Arrumado requisito joao evarisro
</commit_message>
<xml_diff>
--- a/TCC - Monografia/Documentos/Soltos/CaracterísticasAbrasil-2.xlsx
+++ b/TCC - Monografia/Documentos/Soltos/CaracterísticasAbrasil-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="8520" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="7755" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LCP" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="LCP baseline. div. cate. rastre" sheetId="3" r:id="rId3"/>
     <sheet name="Plan1" sheetId="4" r:id="rId4"/>
     <sheet name="Plan4" sheetId="5" r:id="rId5"/>
+    <sheet name="Financeiro" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'LCP base line '!$C$2:$E$50</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="247">
   <si>
     <t>Workshop de Características - Abrasil Express</t>
   </si>
@@ -620,13 +621,171 @@
   </si>
   <si>
     <t>Base line 1</t>
+  </si>
+  <si>
+    <t>Mostrar os vencimentos no dia</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>O sistema deve mostrar quais contas a pagar no dia, semana,mês</t>
+  </si>
+  <si>
+    <t>O sistema deve mostrar as previsões de receita do dia, semana e mês</t>
+  </si>
+  <si>
+    <t>3
+10</t>
+  </si>
+  <si>
+    <t>ver quem ?</t>
+  </si>
+  <si>
+    <t>Coberto</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>O sistema deve cadastrar novas contas</t>
+  </si>
+  <si>
+    <t>1
+2
+5</t>
+  </si>
+  <si>
+    <t>Saber quanto vai entrar de dinheiro até final do mês</t>
+  </si>
+  <si>
+    <t>4
+9</t>
+  </si>
+  <si>
+    <t>Requisitos de Negocio</t>
+  </si>
+  <si>
+    <t>O sitema deve mostrar os devedores</t>
+  </si>
+  <si>
+    <t>6
+7
+8
+14</t>
+  </si>
+  <si>
+    <t>Caracteristica 
+Antecessoras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caracteristicas </t>
+  </si>
+  <si>
+    <t>Requisito Antecessor</t>
+  </si>
+  <si>
+    <t>Regra de Negocio</t>
+  </si>
+  <si>
+    <t>O sistema deve mostrar os resultados financeiros do periodo (D.R.E)</t>
+  </si>
+  <si>
+    <t>Requisito de Sistema</t>
+  </si>
+  <si>
+    <t>Caso De Uso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso De Teste </t>
+  </si>
+  <si>
+    <t>Componente</t>
+  </si>
+  <si>
+    <t>Mostrar resultado financeiro mês</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar Faturamento por mês </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerenciar Contas </t>
+  </si>
+  <si>
+    <t>Requisito Negocio Antecessor</t>
+  </si>
+  <si>
+    <t>1
+2
+3
+5
+7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuário escolher por botão de quer ver contas a vencer no dia, semana ou mês </t>
+  </si>
+  <si>
+    <t>Para cadastar contas é obrigatório ter: 
+Valor, dt vencimento, categorizar em divisão e ter uma descrição(nome)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuário escolher por botão se quer ver as receitas do dia, semana ou mês </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar separado contas fixas de variáveis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar principais receitas divididas por catergorias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve mostrar as contas </t>
+  </si>
+  <si>
+    <t>Filtrar contas por vencimento e por valor</t>
+  </si>
+  <si>
+    <t>O sistema deve mostrar faturamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar faturamento por ano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar atrasados </t>
+  </si>
+  <si>
+    <t>Fazer botão para esquecer conta(como se não contasse mas n sistema(desisido de cobrar)</t>
+  </si>
+  <si>
+    <t>Gestão contas a pagar</t>
+  </si>
+  <si>
+    <t>Cadastrar Contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ver resultado das contas do mês </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ver situação das contas da empresa </t>
+  </si>
+  <si>
+    <t>Gestão contas a Cobrar</t>
+  </si>
+  <si>
+    <t>Ver faturamnto dos outros meses</t>
+  </si>
+  <si>
+    <t>4
+7</t>
+  </si>
+  <si>
+    <t>Caso de uso Antecessor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -742,8 +901,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,6 +971,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -925,7 +1155,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1048,6 +1278,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,6 +1356,69 @@
     <cellStyle name="Título 1" xfId="2" builtinId="16"/>
   </cellStyles>
   <dxfs count="78">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1324,48 +1688,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
@@ -1430,27 +1752,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4300,8 +4601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4641,9 +4942,7 @@
       <c r="B19" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>64</v>
-      </c>
+      <c r="C19" s="27"/>
       <c r="D19" s="14" t="s">
         <v>9</v>
       </c>
@@ -4696,7 +4995,7 @@
         <v>134</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>87</v>
+        <v>199</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>9</v>
@@ -5786,14 +6085,14 @@
     <mergeCell ref="A2:A17"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D17 D36:D41 D50:D58 D60:D65 D76:D1048576 D19:D34 D43:D47 D67:D74">
-    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="Crítico">
-      <formula>NOT(ISERROR(SEARCH("Crítico",D1)))</formula>
+    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="Útil">
+      <formula>NOT(ISERROR(SEARCH("Útil",D1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="Importante">
       <formula>NOT(ISERROR(SEARCH("Importante",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="Útil">
-      <formula>NOT(ISERROR(SEARCH("Útil",D1)))</formula>
+    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="Crítico">
+      <formula>NOT(ISERROR(SEARCH("Crítico",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
@@ -5841,25 +6140,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E17 E19:E41 E43:E48 E50:E65 E67:E1048576">
-    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="Fácil">
-      <formula>NOT(ISERROR(SEARCH("Fácil",E1)))</formula>
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Difícil">
+      <formula>NOT(ISERROR(SEARCH("Difícil",E1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Médio">
       <formula>NOT(ISERROR(SEARCH("Médio",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="Difícil">
-      <formula>NOT(ISERROR(SEARCH("Difícil",E1)))</formula>
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Fácil">
+      <formula>NOT(ISERROR(SEARCH("Fácil",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F17 F19:F41 F43:F48 F50:F65 F67:F1048576">
-    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Alto">
-      <formula>NOT(ISERROR(SEARCH("Alto",F1)))</formula>
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="Baixo">
+      <formula>NOT(ISERROR(SEARCH("Baixo",F1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="Médio">
       <formula>NOT(ISERROR(SEARCH("Médio",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="Baixo">
-      <formula>NOT(ISERROR(SEARCH("Baixo",F1)))</formula>
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Alto">
+      <formula>NOT(ISERROR(SEARCH("Alto",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
@@ -7275,4 +7574,695 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="50" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.5703125" style="49" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="48" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" style="48" customWidth="1"/>
+    <col min="11" max="11" width="47.42578125" style="71" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="48" customWidth="1"/>
+    <col min="14" max="14" width="43.85546875" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="46" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="52" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="62" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="H1" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" s="62" t="s">
+        <v>226</v>
+      </c>
+      <c r="J1" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="L1" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="M1" s="62" t="s">
+        <v>226</v>
+      </c>
+      <c r="N1" s="55" t="s">
+        <v>219</v>
+      </c>
+      <c r="O1" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="P1" s="62" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q1" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="R1" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="S1" s="62" t="s">
+        <v>246</v>
+      </c>
+      <c r="T1" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="U1" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="V1" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="W1" s="55" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="B2" s="57">
+        <v>1</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="59">
+        <v>1</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="67">
+        <v>1</v>
+      </c>
+      <c r="J2" s="67">
+        <v>1</v>
+      </c>
+      <c r="K2" s="70" t="s">
+        <v>228</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="68" t="s">
+        <v>227</v>
+      </c>
+      <c r="N2" s="64" t="s">
+        <v>225</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="73">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="72" t="s">
+        <v>239</v>
+      </c>
+      <c r="R2" s="3"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+    </row>
+    <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="57">
+        <v>2</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="59">
+        <v>2</v>
+      </c>
+      <c r="G3" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="66">
+        <v>2</v>
+      </c>
+      <c r="J3" s="66">
+        <v>2</v>
+      </c>
+      <c r="K3" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="69">
+        <v>4</v>
+      </c>
+      <c r="N3" s="64" t="s">
+        <v>223</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="73">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="72" t="s">
+        <v>243</v>
+      </c>
+      <c r="R3" s="3"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+    </row>
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="57">
+        <v>3</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="F4" s="59">
+        <v>3</v>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>202</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="66">
+        <v>3</v>
+      </c>
+      <c r="J4" s="66">
+        <v>3</v>
+      </c>
+      <c r="K4" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="69">
+        <v>6</v>
+      </c>
+      <c r="N4" s="64" t="s">
+        <v>224</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="73">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="72" t="s">
+        <v>240</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="65"/>
+      <c r="W4" s="65"/>
+    </row>
+    <row r="5" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="57">
+        <v>4</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="59">
+        <v>4</v>
+      </c>
+      <c r="G5" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="66">
+        <v>4</v>
+      </c>
+      <c r="J5" s="66">
+        <v>4</v>
+      </c>
+      <c r="K5" s="70" t="s">
+        <v>231</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="74" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q5" s="72" t="s">
+        <v>241</v>
+      </c>
+      <c r="R5" s="3"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+    </row>
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="57">
+        <v>5</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E6" s="61">
+        <v>11</v>
+      </c>
+      <c r="F6" s="61">
+        <v>5</v>
+      </c>
+      <c r="G6" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="66">
+        <v>4</v>
+      </c>
+      <c r="J6" s="66">
+        <v>5</v>
+      </c>
+      <c r="K6" s="70" t="s">
+        <v>232</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="73">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="72" t="s">
+        <v>242</v>
+      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="65"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="57">
+        <v>6</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E7" s="61">
+        <v>12</v>
+      </c>
+      <c r="F7" s="61">
+        <v>6</v>
+      </c>
+      <c r="G7" s="60" t="s">
+        <v>235</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="66">
+        <v>5</v>
+      </c>
+      <c r="J7" s="66">
+        <v>6</v>
+      </c>
+      <c r="K7" s="70" t="s">
+        <v>234</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="74">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="72" t="s">
+        <v>244</v>
+      </c>
+      <c r="R7" s="3"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="65"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B8" s="57">
+        <v>7</v>
+      </c>
+      <c r="C8" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E8" s="61">
+        <v>13</v>
+      </c>
+      <c r="F8" s="61">
+        <v>7</v>
+      </c>
+      <c r="G8" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="66">
+        <v>6</v>
+      </c>
+      <c r="J8" s="66">
+        <v>7</v>
+      </c>
+      <c r="K8" s="70" t="s">
+        <v>236</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="65"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="57">
+        <v>8</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61">
+        <v>8</v>
+      </c>
+      <c r="G9" s="60"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="66">
+        <v>7</v>
+      </c>
+      <c r="J9" s="66">
+        <v>8</v>
+      </c>
+      <c r="K9" s="70" t="s">
+        <v>237</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="65"/>
+      <c r="W9" s="65"/>
+    </row>
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="57">
+        <v>9</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="66">
+        <v>7</v>
+      </c>
+      <c r="J10" s="66">
+        <v>9</v>
+      </c>
+      <c r="K10" s="70" t="s">
+        <v>238</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="65"/>
+      <c r="W10" s="65"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="57">
+        <v>10</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="65"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="57">
+        <v>11</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="70"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="65"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="57">
+        <v>12</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="65"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="57">
+        <v>13</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="65"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="57">
+        <v>14</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="66"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="65"/>
+      <c r="W15" s="65"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" s="57">
+        <v>15</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="73"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="65"/>
+      <c r="W16" s="65"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>